<commit_message>
Added the function DoubleSinglePrime and SingleDoublePrime
</commit_message>
<xml_diff>
--- a/Record.xlsx
+++ b/Record.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t xml:space="preserve">Condition </t>
   </si>
@@ -46,7 +46,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,14 +79,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -381,122 +399,125 @@
   <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.21875" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="1" max="4" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="3">
+        <f xml:space="preserve"> 10 / 60</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="2">
+        <f>10/60</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1">
         <f>SUM(B3:B8)</f>
-        <v>0</v>
-      </c>
-      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
         <f>SUM(C3:C8)</f>
-        <v>0</v>
-      </c>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>